<commit_message>
Question 2 of exercise 5 completed
</commit_message>
<xml_diff>
--- a/Exercise5Excel.xlsx
+++ b/Exercise5Excel.xlsx
@@ -9,12 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Table 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="6" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="22">
   <si>
     <t>Ivy League Applicants</t>
   </si>
@@ -75,6 +81,21 @@
   </si>
   <si>
     <t>Penn State</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Students</t>
+  </si>
+  <si>
+    <t>Average of Students2</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
   </si>
 </sst>
 </file>
@@ -181,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -216,6 +237,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +262,565 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="NEDER Mohamed El Hocine" refreshedDate="45290.954262500003" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="40">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A2:C42" sheet="Part 1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Students" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="135" maxValue="9567" count="37">
+        <n v="591"/>
+        <n v="9567"/>
+        <n v="542"/>
+        <n v="346"/>
+        <n v="849"/>
+        <n v="552"/>
+        <n v="173"/>
+        <n v="1355"/>
+        <n v="193"/>
+        <n v="615"/>
+        <n v="1579"/>
+        <n v="547"/>
+        <n v="1687"/>
+        <n v="972"/>
+        <n v="234"/>
+        <n v="151"/>
+        <n v="1793"/>
+        <n v="315"/>
+        <n v="618"/>
+        <n v="246"/>
+        <n v="784"/>
+        <n v="316"/>
+        <n v="3155"/>
+        <n v="318"/>
+        <n v="608"/>
+        <n v="561"/>
+        <n v="357"/>
+        <n v="1688"/>
+        <n v="568"/>
+        <n v="632"/>
+        <n v="551"/>
+        <n v="948"/>
+        <n v="1358"/>
+        <n v="135"/>
+        <n v="158"/>
+        <n v="1889"/>
+        <n v="651"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Faculty" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Arts"/>
+        <s v="Physics"/>
+        <s v="Economics"/>
+        <s v="Mathematics"/>
+        <s v="Psychology"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="University" numFmtId="0">
+      <sharedItems count="8">
+        <s v="Yale"/>
+        <s v="Brown"/>
+        <s v="Dartmouth"/>
+        <s v="Harvard"/>
+        <s v="Columbia"/>
+        <s v="Cornell"/>
+        <s v="Princeton"/>
+        <s v="Penn State"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="40">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="4"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="4"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <x v="3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="1"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <x v="3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="4"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <x v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <x v="3"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Average of Students2" fld="0" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Average of Students2" fld="0" subtotal="average" baseField="2" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0">
+      <items count="38">
+        <item x="33"/>
+        <item x="15"/>
+        <item x="34"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item x="19"/>
+        <item x="17"/>
+        <item x="21"/>
+        <item x="23"/>
+        <item x="3"/>
+        <item x="26"/>
+        <item x="2"/>
+        <item x="11"/>
+        <item x="30"/>
+        <item x="5"/>
+        <item x="25"/>
+        <item x="28"/>
+        <item x="0"/>
+        <item x="24"/>
+        <item x="9"/>
+        <item x="18"/>
+        <item x="29"/>
+        <item x="36"/>
+        <item x="20"/>
+        <item x="4"/>
+        <item x="31"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="32"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="27"/>
+        <item x="16"/>
+        <item x="35"/>
+        <item x="22"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,4 +1760,511 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="14">
+        <v>8177</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1022.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14">
+        <v>4877</v>
+      </c>
+      <c r="C5" s="14">
+        <v>609.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="14">
+        <v>7761</v>
+      </c>
+      <c r="C6" s="14">
+        <v>970.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14">
+        <v>15071</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1883.875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="14">
+        <v>4188</v>
+      </c>
+      <c r="C8" s="14">
+        <v>523.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="14">
+        <v>40074</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1001.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14">
+        <v>14127</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2825.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="14">
+        <v>5253</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1050.5999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4965</v>
+      </c>
+      <c r="C6" s="14">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>6247</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1249.4000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2240</v>
+      </c>
+      <c r="C8" s="14">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1887</v>
+      </c>
+      <c r="C9" s="14">
+        <v>377.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2661</v>
+      </c>
+      <c r="C10" s="14">
+        <v>532.20000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2694</v>
+      </c>
+      <c r="C11" s="14">
+        <v>538.79999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="14">
+        <v>40074</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1001.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="4" customWidth="1"/>
+    <col min="18" max="18" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="4" customWidth="1"/>
+    <col min="24" max="26" width="5" customWidth="1"/>
+    <col min="27" max="27" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="4" customWidth="1"/>
+    <col min="34" max="35" width="5" customWidth="1"/>
+    <col min="36" max="36" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="43" width="4" customWidth="1"/>
+    <col min="44" max="44" width="5" customWidth="1"/>
+    <col min="45" max="45" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1358</v>
+      </c>
+      <c r="C5" s="14">
+        <v>972</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1579</v>
+      </c>
+      <c r="E5" s="14">
+        <v>9567</v>
+      </c>
+      <c r="F5" s="14">
+        <v>651</v>
+      </c>
+      <c r="G5" s="14">
+        <v>14127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="14">
+        <v>849</v>
+      </c>
+      <c r="C6" s="14">
+        <v>608</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1688</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1793</v>
+      </c>
+      <c r="F6" s="14">
+        <v>315</v>
+      </c>
+      <c r="G6" s="14">
+        <v>5253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1355</v>
+      </c>
+      <c r="C7" s="14">
+        <v>552</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1889</v>
+      </c>
+      <c r="E7" s="14">
+        <v>618</v>
+      </c>
+      <c r="F7" s="14">
+        <v>551</v>
+      </c>
+      <c r="G7" s="14">
+        <v>4965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14">
+        <v>3155</v>
+      </c>
+      <c r="C8" s="14">
+        <v>542</v>
+      </c>
+      <c r="D8" s="14">
+        <v>316</v>
+      </c>
+      <c r="E8" s="14">
+        <v>547</v>
+      </c>
+      <c r="F8" s="14">
+        <v>1687</v>
+      </c>
+      <c r="G8" s="14">
+        <v>6247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="14">
+        <v>173</v>
+      </c>
+      <c r="C9" s="14">
+        <v>346</v>
+      </c>
+      <c r="D9" s="14">
+        <v>615</v>
+      </c>
+      <c r="E9" s="14">
+        <v>948</v>
+      </c>
+      <c r="F9" s="14">
+        <v>158</v>
+      </c>
+      <c r="G9" s="14">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="14">
+        <v>135</v>
+      </c>
+      <c r="C10" s="14">
+        <v>234</v>
+      </c>
+      <c r="D10" s="14">
+        <v>632</v>
+      </c>
+      <c r="E10" s="14">
+        <v>568</v>
+      </c>
+      <c r="F10" s="14">
+        <v>318</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="14">
+        <v>561</v>
+      </c>
+      <c r="C11" s="14">
+        <v>972</v>
+      </c>
+      <c r="D11" s="14">
+        <v>193</v>
+      </c>
+      <c r="E11" s="14">
+        <v>784</v>
+      </c>
+      <c r="F11" s="14">
+        <v>151</v>
+      </c>
+      <c r="G11" s="14">
+        <v>2661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="14">
+        <v>591</v>
+      </c>
+      <c r="C12" s="14">
+        <v>651</v>
+      </c>
+      <c r="D12" s="14">
+        <v>849</v>
+      </c>
+      <c r="E12" s="14">
+        <v>246</v>
+      </c>
+      <c r="F12" s="14">
+        <v>357</v>
+      </c>
+      <c r="G12" s="14">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="14">
+        <v>8177</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4877</v>
+      </c>
+      <c r="D13" s="14">
+        <v>7761</v>
+      </c>
+      <c r="E13" s="14">
+        <v>15071</v>
+      </c>
+      <c r="F13" s="14">
+        <v>4188</v>
+      </c>
+      <c r="G13" s="14">
+        <v>40074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Question 3 of exercise 5 completed
</commit_message>
<xml_diff>
--- a/Exercise5Excel.xlsx
+++ b/Exercise5Excel.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 1" sheetId="2" r:id="rId2"/>
     <sheet name="Table 2" sheetId="3" r:id="rId3"/>
     <sheet name="Table 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Part 3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
   <si>
     <t>Ivy League Applicants</t>
   </si>
@@ -96,13 +97,49 @@
   </si>
   <si>
     <t>Column Labels</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>QTE</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>Remise</t>
+  </si>
+  <si>
+    <t>Val Remise</t>
+  </si>
+  <si>
+    <t>Total a payer</t>
+  </si>
+  <si>
+    <t>Totale facture:</t>
+  </si>
+  <si>
+    <t>TVA:</t>
+  </si>
+  <si>
+    <t>TTC:</t>
+  </si>
+  <si>
+    <t>Val TVA:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="#,##0.00\ [$DZD]"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +163,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +213,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -198,11 +277,198 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -231,20 +497,85 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -547,7 +878,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -611,7 +942,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -687,7 +1018,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0">
@@ -1100,11 +1431,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1778,7 +2109,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -1789,68 +2120,68 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="12">
         <v>8177</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>1022.125</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>4877</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>609.625</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>7761</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>970.125</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>15071</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="12">
         <v>1883.875</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>4188</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>523.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>40074</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="12">
         <v>1001.85</v>
       </c>
     </row>
@@ -1875,7 +2206,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -1886,101 +2217,101 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="12">
         <v>14127</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>2825.4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>5253</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>1050.5999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>4965</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>993</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>6247</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="12">
         <v>1249.4000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>2240</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>1887</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="12">
         <v>377.4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>2661</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>532.20000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>2694</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="12">
         <v>538.79999999999995</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>40074</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <v>1001.85</v>
       </c>
     </row>
@@ -1993,7 +2324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -2027,15 +2358,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -2058,213 +2389,684 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>1358</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>972</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>1579</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>9567</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>651</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="12">
         <v>14127</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>849</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>608</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>1688</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>1793</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <v>315</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <v>5253</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>1355</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="12">
         <v>552</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>1889</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>618</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <v>551</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <v>4965</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>3155</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>542</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>316</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>547</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="12">
         <v>1687</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <v>6247</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>173</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="12">
         <v>346</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>615</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="12">
         <v>948</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="12">
         <v>158</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="12">
         <v>2240</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>135</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>234</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>632</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="12">
         <v>568</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="12">
         <v>318</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="12">
         <v>1887</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>561</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="12">
         <v>972</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>193</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="12">
         <v>784</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="12">
         <v>151</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <v>2661</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>591</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <v>651</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>849</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="12">
         <v>246</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="12">
         <v>357</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="12">
         <v>2694</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>8177</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <v>4877</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <v>7761</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="12">
         <v>15071</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="12">
         <v>4188</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <v>40074</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27">
+        <v>120</v>
+      </c>
+      <c r="C2" s="15">
+        <v>3</v>
+      </c>
+      <c r="D2" s="27">
+        <f>B2*C2</f>
+        <v>360</v>
+      </c>
+      <c r="E2" s="30">
+        <f>IF(D2&lt;100,0,IF(D2&lt;=999,0.05,0.1))</f>
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="27">
+        <f>D2*E2</f>
+        <v>18</v>
+      </c>
+      <c r="G2" s="25">
+        <f>D2-F2</f>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28">
+        <v>56</v>
+      </c>
+      <c r="C3" s="16">
+        <v>5</v>
+      </c>
+      <c r="D3" s="28">
+        <f t="shared" ref="D3:D15" si="0">B3*C3</f>
+        <v>280</v>
+      </c>
+      <c r="E3" s="31">
+        <f t="shared" ref="E3:E15" si="1">IF(D3&lt;100,0,IF(D3&lt;=999,0.05,0.1))</f>
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="28">
+        <f t="shared" ref="F3:F15" si="2">D3*E3</f>
+        <v>14</v>
+      </c>
+      <c r="G3" s="24">
+        <f t="shared" ref="G3:G15" si="3">D3-F3</f>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27">
+        <v>70</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="27">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="E4" s="30">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="27">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="3"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="28">
+        <v>430</v>
+      </c>
+      <c r="C5" s="16">
+        <v>7</v>
+      </c>
+      <c r="D5" s="28">
+        <f t="shared" si="0"/>
+        <v>3010</v>
+      </c>
+      <c r="E5" s="31">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="28">
+        <f t="shared" si="2"/>
+        <v>301</v>
+      </c>
+      <c r="G5" s="24">
+        <f t="shared" si="3"/>
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="21">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27">
+        <v>230</v>
+      </c>
+      <c r="C6" s="15">
+        <v>23</v>
+      </c>
+      <c r="D6" s="27">
+        <f t="shared" si="0"/>
+        <v>5290</v>
+      </c>
+      <c r="E6" s="30">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="27">
+        <f t="shared" si="2"/>
+        <v>529</v>
+      </c>
+      <c r="G6" s="25">
+        <f t="shared" si="3"/>
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="28">
+        <v>10</v>
+      </c>
+      <c r="C7" s="16">
+        <v>2</v>
+      </c>
+      <c r="D7" s="28">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E7" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="24">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="21">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
+        <v>8</v>
+      </c>
+      <c r="D8" s="27">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E8" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="25">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="28">
+        <v>5040</v>
+      </c>
+      <c r="C9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="28">
+        <f t="shared" si="0"/>
+        <v>5040</v>
+      </c>
+      <c r="E9" s="31">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="28">
+        <f t="shared" si="2"/>
+        <v>504</v>
+      </c>
+      <c r="G9" s="24">
+        <f t="shared" si="3"/>
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="21">
+        <v>9</v>
+      </c>
+      <c r="B10" s="27">
+        <v>1200</v>
+      </c>
+      <c r="C10" s="15">
+        <v>3</v>
+      </c>
+      <c r="D10" s="27">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+      <c r="E10" s="30">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="27">
+        <f t="shared" si="2"/>
+        <v>360</v>
+      </c>
+      <c r="G10" s="25">
+        <f t="shared" si="3"/>
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28">
+        <v>480</v>
+      </c>
+      <c r="C11" s="16">
+        <v>4</v>
+      </c>
+      <c r="D11" s="28">
+        <f t="shared" si="0"/>
+        <v>1920</v>
+      </c>
+      <c r="E11" s="31">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="28">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="G11" s="24">
+        <f t="shared" si="3"/>
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <v>11</v>
+      </c>
+      <c r="B12" s="27">
+        <v>33</v>
+      </c>
+      <c r="C12" s="15">
+        <v>5</v>
+      </c>
+      <c r="D12" s="27">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="E12" s="30">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="27">
+        <f t="shared" si="2"/>
+        <v>8.25</v>
+      </c>
+      <c r="G12" s="25">
+        <f t="shared" si="3"/>
+        <v>156.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
+        <v>12</v>
+      </c>
+      <c r="B13" s="28">
+        <v>1200</v>
+      </c>
+      <c r="C13" s="16">
+        <v>2</v>
+      </c>
+      <c r="D13" s="28">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="E13" s="31">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="28">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="G13" s="24">
+        <f t="shared" si="3"/>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="27">
+        <v>15</v>
+      </c>
+      <c r="C14" s="15">
+        <v>10</v>
+      </c>
+      <c r="D14" s="27">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="E14" s="30">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="27">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="G14" s="25">
+        <f t="shared" si="3"/>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="23">
+        <v>14</v>
+      </c>
+      <c r="B15" s="29">
+        <v>24</v>
+      </c>
+      <c r="C15" s="20">
+        <v>5</v>
+      </c>
+      <c r="D15" s="29">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="E15" s="32">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="29">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G15" s="26">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="34"/>
+      <c r="G17" s="39">
+        <f>SUM(G2:G15)</f>
+        <v>20348.25</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="41">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="40">
+        <f>G17*G18</f>
+        <v>3866.1675</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="42">
+        <f>G17+G19</f>
+        <v>24214.4175</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Question 4 of exercise 5 completed
</commit_message>
<xml_diff>
--- a/Exercise5Excel.xlsx
+++ b/Exercise5Excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,11 @@
     <sheet name="Table 2" sheetId="3" r:id="rId3"/>
     <sheet name="Table 3" sheetId="4" r:id="rId4"/>
     <sheet name="Part 3" sheetId="5" r:id="rId5"/>
+    <sheet name="Part 4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="36">
   <si>
     <t>Ivy League Applicants</t>
   </si>
@@ -131,13 +132,22 @@
   <si>
     <t>Val TVA:</t>
   </si>
+  <si>
+    <t>Time(s)</t>
+  </si>
+  <si>
+    <t>Distance (m)</t>
+  </si>
+  <si>
+    <t>Speed (m/s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="#,##0.00\ [$DZD]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$DZD]"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -188,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +241,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -463,12 +479,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -502,12 +605,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -529,16 +626,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,6 +646,16 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -568,10 +675,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,6 +723,1949 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speed/time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Part 4'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speed (m/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Part 4'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Part 4'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2222222222222214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D6AB-489C-B535-021C7EC47688}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="250577856"/>
+        <c:axId val="250585344"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="250577856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="250585344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="250585344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="250577856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speed/Distance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Part 4'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distance (m)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Part 4'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Part 4'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2222222222222214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B0E8-4027-8B15-94498104F071}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="135597568"/>
+        <c:axId val="135603392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="135597568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="135603392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="135603392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="135597568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="34" name="Chart 33"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="35" name="Chart 34"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1431,11 +3504,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2604,8 +4677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="I14:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2619,442 +4692,442 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="25">
         <v>120</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="13">
         <v>3</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="25">
         <f>B2*C2</f>
         <v>360</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="28">
         <f>IF(D2&lt;100,0,IF(D2&lt;=999,0.05,0.1))</f>
         <v>0.05</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="25">
         <f>D2*E2</f>
         <v>18</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="23">
         <f>D2-F2</f>
         <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="22">
+      <c r="A3" s="20">
         <v>2</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="26">
         <v>56</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="14">
         <v>5</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="26">
         <f t="shared" ref="D3:D15" si="0">B3*C3</f>
         <v>280</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="29">
         <f t="shared" ref="E3:E15" si="1">IF(D3&lt;100,0,IF(D3&lt;=999,0.05,0.1))</f>
         <v>0.05</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="26">
         <f t="shared" ref="F3:F15" si="2">D3*E3</f>
         <v>14</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="22">
         <f t="shared" ref="G3:G15" si="3">D3-F3</f>
         <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="21">
+      <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="25">
         <v>70</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>2</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="25">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="28">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="25">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="23">
         <f t="shared" si="3"/>
         <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <v>430</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="14">
         <v>7</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="26">
         <f t="shared" si="0"/>
         <v>3010</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="29">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="26">
         <f t="shared" si="2"/>
         <v>301</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="22">
         <f t="shared" si="3"/>
         <v>2709</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="21">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="25">
         <v>230</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="13">
         <v>23</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="25">
         <f t="shared" si="0"/>
         <v>5290</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="25">
         <f t="shared" si="2"/>
         <v>529</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="23">
         <f t="shared" si="3"/>
         <v>4761</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="20">
         <v>6</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="26">
         <v>10</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="14">
         <v>2</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="26">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="22">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
+      <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="25">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="13">
         <v>8</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="23">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="26">
         <v>5040</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <v>1</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="26">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="29">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="26">
         <f t="shared" si="2"/>
         <v>504</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="22">
         <f t="shared" si="3"/>
         <v>4536</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="25">
         <v>1200</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <v>3</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="25">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="28">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <f t="shared" si="2"/>
         <v>360</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="23">
         <f t="shared" si="3"/>
         <v>3240</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="20">
         <v>10</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="26">
         <v>480</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <v>4</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="26">
         <f t="shared" si="0"/>
         <v>1920</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="29">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="26">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="22">
         <f t="shared" si="3"/>
         <v>1728</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
+      <c r="A12" s="19">
         <v>11</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="25">
         <v>33</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="13">
         <v>5</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="25">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="28">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="25">
         <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="23">
         <f t="shared" si="3"/>
         <v>156.75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="22">
+      <c r="A13" s="20">
         <v>12</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="26">
         <v>1200</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <v>2</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="26">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="29">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="26">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="22">
         <f t="shared" si="3"/>
         <v>2160</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
+      <c r="A14" s="19">
         <v>13</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="25">
         <v>15</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="13">
         <v>10</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="25">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="28">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="25">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="23">
         <f t="shared" si="3"/>
         <v>142.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23">
+      <c r="A15" s="21">
         <v>14</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="27">
         <v>24</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="18">
         <v>5</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="27">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="30">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="27">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="24">
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="39">
+      <c r="F17" s="38"/>
+      <c r="G17" s="31">
         <f>SUM(G2:G15)</f>
         <v>20348.25</v>
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="41">
+      <c r="F18" s="40"/>
+      <c r="G18" s="33">
         <v>0.19</v>
       </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="40">
+      <c r="F19" s="40"/>
+      <c r="G19" s="32">
         <f>G17*G18</f>
         <v>3866.1675</v>
       </c>
     </row>
     <row r="20" spans="5:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="42">
+      <c r="F20" s="42"/>
+      <c r="G20" s="34">
         <f>G17+G19</f>
         <v>24214.4175</v>
       </c>
@@ -3069,4 +5142,157 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="46">
+        <v>1</v>
+      </c>
+      <c r="B2" s="46">
+        <v>5</v>
+      </c>
+      <c r="C2" s="47">
+        <f>B2/A2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="48">
+        <v>2</v>
+      </c>
+      <c r="B3" s="48">
+        <v>10</v>
+      </c>
+      <c r="C3" s="49">
+        <f t="shared" ref="C3:C11" si="0">B3/A3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="46">
+        <v>3</v>
+      </c>
+      <c r="B4" s="46">
+        <v>17</v>
+      </c>
+      <c r="C4" s="47">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="48">
+        <v>4</v>
+      </c>
+      <c r="B5" s="48">
+        <v>27</v>
+      </c>
+      <c r="C5" s="49">
+        <f t="shared" si="0"/>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="46">
+        <v>5</v>
+      </c>
+      <c r="B6" s="46">
+        <v>37</v>
+      </c>
+      <c r="C6" s="47">
+        <f t="shared" si="0"/>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="48">
+        <v>6</v>
+      </c>
+      <c r="B7" s="48">
+        <v>49</v>
+      </c>
+      <c r="C7" s="49">
+        <f t="shared" si="0"/>
+        <v>8.1666666666666661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="46">
+        <v>7</v>
+      </c>
+      <c r="B8" s="46">
+        <v>63</v>
+      </c>
+      <c r="C8" s="47">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="48">
+        <v>8</v>
+      </c>
+      <c r="B9" s="48">
+        <v>75</v>
+      </c>
+      <c r="C9" s="49">
+        <f t="shared" si="0"/>
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="46">
+        <v>9</v>
+      </c>
+      <c r="B10" s="46">
+        <v>83</v>
+      </c>
+      <c r="C10" s="47">
+        <f t="shared" si="0"/>
+        <v>9.2222222222222214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="50">
+        <v>10</v>
+      </c>
+      <c r="B11" s="50">
+        <v>91</v>
+      </c>
+      <c r="C11" s="51">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding thick outside borders to the main table in part 3
</commit_message>
<xml_diff>
--- a/Exercise5Excel.xlsx
+++ b/Exercise5Excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -248,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -561,6 +561,66 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -617,18 +677,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -651,30 +699,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -702,6 +726,42 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3504,11 +3564,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -4677,8 +4737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="I14:J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4715,419 +4775,419 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+      <c r="A2" s="46">
         <v>1</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="19">
         <v>120</v>
       </c>
       <c r="C2" s="13">
         <v>3</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="19">
         <f>B2*C2</f>
         <v>360</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="22">
         <f>IF(D2&lt;100,0,IF(D2&lt;=999,0.05,0.1))</f>
         <v>0.05</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="19">
         <f>D2*E2</f>
         <v>18</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="47">
         <f>D2-F2</f>
         <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
+      <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="20">
         <v>56</v>
       </c>
       <c r="C3" s="14">
         <v>5</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="20">
         <f t="shared" ref="D3:D15" si="0">B3*C3</f>
         <v>280</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="23">
         <f t="shared" ref="E3:E15" si="1">IF(D3&lt;100,0,IF(D3&lt;=999,0.05,0.1))</f>
         <v>0.05</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="20">
         <f t="shared" ref="F3:F15" si="2">D3*E3</f>
         <v>14</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="49">
         <f t="shared" ref="G3:G15" si="3">D3-F3</f>
         <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
+      <c r="A4" s="46">
         <v>3</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="19">
         <v>70</v>
       </c>
       <c r="C4" s="13">
         <v>2</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="19">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="22">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="19">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="47">
         <f t="shared" si="3"/>
         <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="20">
+      <c r="A5" s="48">
         <v>4</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="20">
         <v>430</v>
       </c>
       <c r="C5" s="14">
         <v>7</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="20">
         <f t="shared" si="0"/>
         <v>3010</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="23">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="20">
         <f t="shared" si="2"/>
         <v>301</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="49">
         <f t="shared" si="3"/>
         <v>2709</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
+      <c r="A6" s="46">
         <v>5</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="19">
         <v>230</v>
       </c>
       <c r="C6" s="13">
         <v>23</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="19">
         <f t="shared" si="0"/>
         <v>5290</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="22">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="19">
         <f t="shared" si="2"/>
         <v>529</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="47">
         <f t="shared" si="3"/>
         <v>4761</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="20">
+      <c r="A7" s="48">
         <v>6</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="20">
         <v>10</v>
       </c>
       <c r="C7" s="14">
         <v>2</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="20">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="49">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="A8" s="46">
         <v>7</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="19">
         <v>5</v>
       </c>
       <c r="C8" s="13">
         <v>8</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="19">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="47">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="48">
         <v>8</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="20">
         <v>5040</v>
       </c>
       <c r="C9" s="14">
         <v>1</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="20">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="23">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="20">
         <f t="shared" si="2"/>
         <v>504</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="49">
         <f t="shared" si="3"/>
         <v>4536</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+      <c r="A10" s="46">
         <v>9</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="19">
         <v>1200</v>
       </c>
       <c r="C10" s="13">
         <v>3</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="19">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="22">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="19">
         <f t="shared" si="2"/>
         <v>360</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="47">
         <f t="shared" si="3"/>
         <v>3240</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
+      <c r="A11" s="48">
         <v>10</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="20">
         <v>480</v>
       </c>
       <c r="C11" s="14">
         <v>4</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="20">
         <f t="shared" si="0"/>
         <v>1920</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="23">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="20">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="49">
         <f t="shared" si="3"/>
         <v>1728</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="A12" s="46">
         <v>11</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="19">
         <v>33</v>
       </c>
       <c r="C12" s="13">
         <v>5</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="19">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="22">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="19">
         <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="47">
         <f t="shared" si="3"/>
         <v>156.75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
+      <c r="A13" s="48">
         <v>12</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="20">
         <v>1200</v>
       </c>
       <c r="C13" s="14">
         <v>2</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="20">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="23">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="20">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="49">
         <f t="shared" si="3"/>
         <v>2160</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
+      <c r="A14" s="46">
         <v>13</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="19">
         <v>15</v>
       </c>
       <c r="C14" s="13">
         <v>10</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="19">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="22">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="19">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="47">
         <f t="shared" si="3"/>
         <v>142.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="21">
+      <c r="A15" s="50">
         <v>14</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="21">
         <v>24</v>
       </c>
       <c r="C15" s="18">
         <v>5</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="21">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="24">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="21">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="51">
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="31">
+      <c r="F17" s="41"/>
+      <c r="G17" s="25">
         <f>SUM(G2:G15)</f>
         <v>20348.25</v>
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="33">
+      <c r="F18" s="43"/>
+      <c r="G18" s="27">
         <v>0.19</v>
       </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="32">
+      <c r="F19" s="43"/>
+      <c r="G19" s="26">
         <f>G17*G18</f>
         <v>3866.1675</v>
       </c>
     </row>
     <row r="20" spans="5:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="34">
+      <c r="F20" s="45"/>
+      <c r="G20" s="28">
         <f>G17+G19</f>
         <v>24214.4175</v>
       </c>
@@ -5148,7 +5208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -5160,132 +5220,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="46">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="32">
         <v>5</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="33">
         <f>B2/A2</f>
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="48">
+      <c r="A3" s="34">
         <v>2</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="34">
         <v>10</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="35">
         <f t="shared" ref="C3:C11" si="0">B3/A3</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="46">
+      <c r="A4" s="32">
         <v>3</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="32">
         <v>17</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="33">
         <f t="shared" si="0"/>
         <v>5.666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="48">
+      <c r="A5" s="34">
         <v>4</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="34">
         <v>27</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="35">
         <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="46">
+      <c r="A6" s="32">
         <v>5</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="32">
         <v>37</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="33">
         <f t="shared" si="0"/>
         <v>7.4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="48">
+      <c r="A7" s="34">
         <v>6</v>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="34">
         <v>49</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="35">
         <f t="shared" si="0"/>
         <v>8.1666666666666661</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="46">
+      <c r="A8" s="32">
         <v>7</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="32">
         <v>63</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="33">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="48">
+      <c r="A9" s="34">
         <v>8</v>
       </c>
-      <c r="B9" s="48">
+      <c r="B9" s="34">
         <v>75</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="35">
         <f t="shared" si="0"/>
         <v>9.375</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="46">
+      <c r="A10" s="32">
         <v>9</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="32">
         <v>83</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="33">
         <f t="shared" si="0"/>
         <v>9.2222222222222214</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="50">
+      <c r="A11" s="36">
         <v>10</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B11" s="36">
         <v>91</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="37">
         <f t="shared" si="0"/>
         <v>9.1</v>
       </c>

</xml_diff>